<commit_message>
Bugfix DiGraph in AST drops nodes
Problem: adding nodes to networkX DiGraph was essentially doing a set opeation on similar nodes. eg; multiple f_tokens with the same value say 1 or "SPAM" were  being dropped so a function expressed =SUM(1, 1, 1) would return the value 1 not 3.

Fix: f_tokens now have a uuid to ensure unique. Currently using __repr__() for comparison/equality.
Co-Authored-By: Bradley van Ree <bradbase@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/resources/CONCAT.xlsx
+++ b/tests/resources/CONCAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradb\Documents\Python\koala_xlcalculator\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372AD866-27C3-46C7-95BF-FA38842A0F44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C67DFD-5AF3-4B45-ADB0-95C0F65A7283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="158" windowWidth="21480" windowHeight="12742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="158" windowWidth="21480" windowHeight="12742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -472,6 +472,12 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" t="str">
+        <f>_xlfn.CONCAT("SPAM", " ", A1:B2, "SPAM", " ")</f>
+        <v xml:space="preserve">SPAM SPAMSPAMSPAMSPAMSPAM 1234 SPAM SPAMSPAMSPAM </v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>